<commit_message>
insert constant for group
</commit_message>
<xml_diff>
--- a/testspec/powertest.xlsx
+++ b/testspec/powertest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Test Design</t>
   </si>
@@ -69,9 +69,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>U</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - Driver A exists in system
  - Valid value of Driver A is 1
  - setting.ADAS_FCW_ENABLE = 1 in DeviceInfo table </t>
@@ -99,6 +96,9 @@
   <si>
     <t xml:space="preserve">Receive On Setting message 
 </t>
+  </si>
+  <si>
+    <t>OK</t>
   </si>
 </sst>
 </file>
@@ -200,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -275,6 +275,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -284,7 +335,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -313,6 +364,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -397,23 +449,29 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="2" fillId="7" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="12" fontId="2" fillId="7" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="12" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1006,42 +1064,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:I17"/>
+  <dimension ref="A3:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:H17"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" ht="21">
-      <c r="A5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+    <row r="3" spans="1:9" s="12" customFormat="1"/>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="21">
-      <c r="A6" s="5"/>
+      <c r="A6" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -1049,165 +1097,169 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" ht="135">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:9" ht="21">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" ht="135">
+      <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="15">
-        <v>1</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="43"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="16"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="44"/>
+      <c r="A9" s="16">
+        <v>1</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="44" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="16"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="44"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="16"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="44"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="45"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="17"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="24"/>
       <c r="G12" s="24"/>
       <c r="H12" s="42"/>
       <c r="I12" s="45"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="25">
-        <v>2</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="43"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="46"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="26"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="44"/>
+      <c r="A14" s="26">
+        <v>2</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="44" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="26"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="44"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="45"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="26"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="44"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="27"/>
@@ -1220,28 +1272,39 @@
       <c r="H17" s="42"/>
       <c r="I17" s="45"/>
     </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="28"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="46"/>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H13:H17"/>
-    <mergeCell ref="I13:I17"/>
-    <mergeCell ref="G8:G12"/>
-    <mergeCell ref="H8:H12"/>
-    <mergeCell ref="I8:I12"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="G13:G17"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="D13:D17"/>
-    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="H14:H18"/>
+    <mergeCell ref="I14:I18"/>
+    <mergeCell ref="G9:G13"/>
+    <mergeCell ref="H9:H13"/>
+    <mergeCell ref="I9:I13"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="G14:G18"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="D9:D13"/>
+    <mergeCell ref="E9:E13"/>
+    <mergeCell ref="F9:F13"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="D14:D18"/>
+    <mergeCell ref="E14:E18"/>
   </mergeCells>
-  <conditionalFormatting sqref="H8">
+  <conditionalFormatting sqref="H9">
     <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
       <formula>"Cancel"</formula>
     </cfRule>
@@ -1261,7 +1324,7 @@
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
+  <conditionalFormatting sqref="H9">
     <cfRule type="cellIs" dxfId="19" priority="24" stopIfTrue="1" operator="equal">
       <formula>"B"</formula>
     </cfRule>
@@ -1272,21 +1335,21 @@
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
+  <conditionalFormatting sqref="H9">
     <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="U">
-      <formula>NOT(ISERROR(SEARCH("U",H8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("U",H9)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="15" priority="21" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("N/A",H9)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="NG">
-      <formula>NOT(ISERROR(SEARCH("NG",H8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NG",H9)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",H8)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OK",H9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
+  <conditionalFormatting sqref="H14">
     <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Cancel"</formula>
     </cfRule>
@@ -1306,7 +1369,7 @@
       <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
+  <conditionalFormatting sqref="H14">
     <cfRule type="cellIs" dxfId="6" priority="11" stopIfTrue="1" operator="equal">
       <formula>"B"</formula>
     </cfRule>
@@ -1317,28 +1380,28 @@
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
+  <conditionalFormatting sqref="H14">
     <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="U">
-      <formula>NOT(ISERROR(SEARCH("U",H13)))</formula>
+      <formula>NOT(ISERROR(SEARCH("U",H14)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="8" operator="containsText" text="N/A">
-      <formula>NOT(ISERROR(SEARCH("N/A",H13)))</formula>
+      <formula>NOT(ISERROR(SEARCH("N/A",H14)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="9" operator="containsText" text="NG">
-      <formula>NOT(ISERROR(SEARCH("NG",H13)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NG",H14)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="10" operator="containsText" text="OK">
-      <formula>NOT(ISERROR(SEARCH("OK",H13)))</formula>
+      <formula>NOT(ISERROR(SEARCH("OK",H14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
       <formula1>"Expected case, Unexpected case"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5">
       <formula1>"Usual, Rare, Combination"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8 H13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9 H14">
       <formula1>"OK,NG,U,Block,N/A,NT,Cancel"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>